<commit_message>
Previo segunda revision articulo
</commit_message>
<xml_diff>
--- a/tablas/central.xlsx
+++ b/tablas/central.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,13 +16,14 @@
     <sheet name="Cuadro2_si_pre2" sheetId="7" r:id="rId7"/>
     <sheet name="Cuadro2_si_si" sheetId="8" r:id="rId8"/>
     <sheet name="cuadro3_pre" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet2" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="100">
   <si>
     <t>N_sujeto</t>
   </si>
@@ -255,22 +256,85 @@
     <t>PDCL</t>
   </si>
   <si>
-    <t>t wilcox</t>
-  </si>
-  <si>
     <t>W</t>
   </si>
   <si>
     <t>p</t>
+  </si>
+  <si>
+    <t>U mann</t>
+  </si>
+  <si>
+    <t>Int_0</t>
+  </si>
+  <si>
+    <t>int_f</t>
+  </si>
+  <si>
+    <t>diff</t>
+  </si>
+  <si>
+    <t>t Welch</t>
+  </si>
+  <si>
+    <t>Escol.</t>
+  </si>
+  <si>
+    <t>Sueño [s]</t>
+  </si>
+  <si>
+    <t>MOR [%]</t>
+  </si>
+  <si>
+    <t>MOR [s]</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>m1</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>int_0</t>
+  </si>
+  <si>
+    <t>dF</t>
+  </si>
+  <si>
+    <t>sueño hh</t>
+  </si>
+  <si>
+    <t>sueño mm</t>
+  </si>
+  <si>
+    <t>sueño ss</t>
+  </si>
+  <si>
+    <t>mor hh</t>
+  </si>
+  <si>
+    <t>mor mm</t>
+  </si>
+  <si>
+    <t>mor ss</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000000"/>
+    <numFmt numFmtId="174" formatCode="0.0%"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -333,7 +397,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -424,6 +488,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -439,7 +509,7 @@
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -567,16 +637,49 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1484,6 +1587,20 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
@@ -3834,16 +3951,16 @@
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="J24" s="63" t="s">
+      <c r="J24" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="K24" s="63"/>
-      <c r="L24" s="63"/>
-      <c r="N24" s="63" t="s">
+      <c r="K24" s="65"/>
+      <c r="L24" s="65"/>
+      <c r="N24" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="O24" s="63"/>
-      <c r="P24" s="63"/>
+      <c r="O24" s="65"/>
+      <c r="P24" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3860,10 +3977,13 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J16"/>
+      <selection activeCell="J10" sqref="J10:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="9.140625" style="67"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="31"/>
@@ -3888,7 +4008,7 @@
       <c r="H1" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="66" t="s">
         <v>56</v>
       </c>
       <c r="J1" s="46" t="s">
@@ -3929,7 +4049,7 @@
       <c r="H3">
         <v>18</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="67">
         <v>0</v>
       </c>
       <c r="J3">
@@ -3959,7 +4079,7 @@
       <c r="H4">
         <v>19</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="67">
         <v>0</v>
       </c>
       <c r="J4">
@@ -3989,7 +4109,7 @@
       <c r="H5">
         <v>29</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="67">
         <v>1</v>
       </c>
       <c r="J5">
@@ -4019,7 +4139,7 @@
       <c r="H6">
         <v>15</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="67">
         <v>0</v>
       </c>
       <c r="J6">
@@ -4052,7 +4172,7 @@
         <f t="shared" si="0"/>
         <v>20.25</v>
       </c>
-      <c r="I7" s="44">
+      <c r="I7" s="68">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
@@ -4087,7 +4207,7 @@
         <f t="shared" si="1"/>
         <v>6.0759087111860612</v>
       </c>
-      <c r="I8" s="44">
+      <c r="I8" s="68">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
@@ -4129,7 +4249,7 @@
       <c r="H10">
         <v>22</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="67">
         <v>1</v>
       </c>
       <c r="J10">
@@ -4159,7 +4279,7 @@
       <c r="H11">
         <v>20</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="67">
         <v>0</v>
       </c>
       <c r="J11">
@@ -4189,7 +4309,7 @@
       <c r="H12">
         <v>20</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="67">
         <v>0</v>
       </c>
       <c r="J12">
@@ -4216,7 +4336,10 @@
       <c r="G13" s="35">
         <v>29</v>
       </c>
-      <c r="I13">
+      <c r="H13" t="s">
+        <v>88</v>
+      </c>
+      <c r="I13" s="67">
         <v>0</v>
       </c>
       <c r="J13">
@@ -4246,7 +4369,7 @@
       <c r="H14">
         <v>20</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="67">
         <v>0</v>
       </c>
       <c r="J14">
@@ -4279,7 +4402,7 @@
         <f t="shared" si="2"/>
         <v>20.5</v>
       </c>
-      <c r="I15" s="45">
+      <c r="I15" s="69">
         <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
@@ -4314,7 +4437,7 @@
         <f t="shared" ref="H16:J16" si="3">STDEV(H10:H14)</f>
         <v>1</v>
       </c>
-      <c r="I16" s="45">
+      <c r="I16" s="69">
         <f t="shared" si="3"/>
         <v>0.44721359549995793</v>
       </c>
@@ -4330,10 +4453,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF20"/>
+  <dimension ref="A1:AF38"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AD4" sqref="AD4"/>
+    <sheetView topLeftCell="S19" workbookViewId="0">
+      <selection activeCell="AD30" sqref="AD30:AD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4474,26 +4597,26 @@
         <v>36</v>
       </c>
       <c r="L3" s="48">
-        <f t="shared" ref="L3:L18" si="2">E3-J3*60*60-K3*60</f>
+        <f>E3-J3*60*60-K3*60</f>
         <v>25.779999999998836</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N18" si="3">J3</f>
+        <f t="shared" ref="N3:N18" si="2">J3</f>
         <v>8</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O18" si="4">INT(K3/4)*4</f>
+        <f t="shared" ref="O3:O18" si="3">INT(K3/4)*4</f>
         <v>36</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R18" si="5">N3*60*60+O3*60+P3</f>
+        <f t="shared" ref="R3:R18" si="4">N3*60*60+O3*60+P3</f>
         <v>30960</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S14" si="6">R3*C3</f>
+        <f t="shared" ref="S3:S14" si="5">R3*C3</f>
         <v>15851520</v>
       </c>
       <c r="U3">
@@ -4503,19 +4626,19 @@
         <v>127</v>
       </c>
       <c r="X3">
-        <f t="shared" ref="X3:X6" si="7">W3*U3</f>
+        <f t="shared" ref="X3:X6" si="6">W3*U3</f>
         <v>3810</v>
       </c>
       <c r="Z3">
-        <f t="shared" ref="Z3:Z18" si="8">INT(X3/(60*60))</f>
+        <f t="shared" ref="Z3:Z18" si="7">INT(X3/(60*60))</f>
         <v>1</v>
       </c>
       <c r="AA3">
-        <f t="shared" ref="AA3:AA18" si="9">INT((X3-60*60*Z3)/60)</f>
+        <f t="shared" ref="AA3:AA18" si="8">INT((X3-60*60*Z3)/60)</f>
         <v>3</v>
       </c>
       <c r="AB3">
-        <f t="shared" ref="AB3:AB18" si="10">X3-Z3*60*60-AA3*60</f>
+        <f t="shared" ref="AB3:AB18" si="9">X3-Z3*60*60-AA3*60</f>
         <v>30</v>
       </c>
       <c r="AD3" s="52">
@@ -4523,7 +4646,7 @@
         <v>0.12306201550387597</v>
       </c>
       <c r="AF3" s="56">
-        <f t="shared" ref="AF3:AF18" si="11">X3*C3</f>
+        <f t="shared" ref="AF3:AF18" si="10">X3*C3</f>
         <v>1950720</v>
       </c>
     </row>
@@ -4559,26 +4682,26 @@
         <v>33</v>
       </c>
       <c r="L4" s="48">
+        <f t="shared" ref="L3:L18" si="11">E4-J4*60*60-K4*60</f>
+        <v>59.110000000000582</v>
+      </c>
+      <c r="N4">
         <f t="shared" si="2"/>
-        <v>59.110000000000582</v>
-      </c>
-      <c r="N4">
+        <v>7</v>
+      </c>
+      <c r="O4">
         <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="O4">
+        <v>32</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="R4">
         <f t="shared" si="4"/>
-        <v>32</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="R4">
+        <v>27120</v>
+      </c>
+      <c r="S4">
         <f t="shared" si="5"/>
-        <v>27120</v>
-      </c>
-      <c r="S4">
-        <f t="shared" si="6"/>
         <v>13885440</v>
       </c>
       <c r="U4">
@@ -4588,19 +4711,19 @@
         <v>171</v>
       </c>
       <c r="X4">
+        <f t="shared" si="6"/>
+        <v>5130</v>
+      </c>
+      <c r="Z4">
         <f t="shared" si="7"/>
-        <v>5130</v>
-      </c>
-      <c r="Z4">
+        <v>1</v>
+      </c>
+      <c r="AA4">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="AA4">
+        <v>25</v>
+      </c>
+      <c r="AB4">
         <f t="shared" si="9"/>
-        <v>25</v>
-      </c>
-      <c r="AB4">
-        <f t="shared" si="10"/>
         <v>30</v>
       </c>
       <c r="AD4" s="52">
@@ -4608,7 +4731,7 @@
         <v>0.18915929203539822</v>
       </c>
       <c r="AF4" s="56">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>2626560</v>
       </c>
     </row>
@@ -4644,26 +4767,26 @@
         <v>35</v>
       </c>
       <c r="L5" s="48">
+        <f t="shared" si="11"/>
+        <v>20.430000000000291</v>
+      </c>
+      <c r="N5">
         <f t="shared" si="2"/>
-        <v>20.430000000000291</v>
-      </c>
-      <c r="N5">
+        <v>8</v>
+      </c>
+      <c r="O5">
         <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="O5">
+        <v>32</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="R5">
         <f t="shared" si="4"/>
-        <v>32</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="R5">
+        <v>30720</v>
+      </c>
+      <c r="S5">
         <f t="shared" si="5"/>
-        <v>30720</v>
-      </c>
-      <c r="S5">
-        <f t="shared" si="6"/>
         <v>15728640</v>
       </c>
       <c r="U5">
@@ -4673,19 +4796,19 @@
         <v>166</v>
       </c>
       <c r="X5">
+        <f t="shared" si="6"/>
+        <v>4980</v>
+      </c>
+      <c r="Z5">
         <f t="shared" si="7"/>
-        <v>4980</v>
-      </c>
-      <c r="Z5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="AA5">
+        <v>23</v>
+      </c>
+      <c r="AB5">
         <f t="shared" si="9"/>
-        <v>23</v>
-      </c>
-      <c r="AB5">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AD5" s="52">
@@ -4694,7 +4817,7 @@
       </c>
       <c r="AE5" s="50"/>
       <c r="AF5" s="56">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>2549760</v>
       </c>
     </row>
@@ -4730,26 +4853,26 @@
         <v>37</v>
       </c>
       <c r="L6" s="48">
+        <f t="shared" si="11"/>
+        <v>59.459999999999127</v>
+      </c>
+      <c r="N6">
         <f t="shared" si="2"/>
-        <v>59.459999999999127</v>
-      </c>
-      <c r="N6">
+        <v>4</v>
+      </c>
+      <c r="O6">
         <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="O6">
+        <v>36</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="R6">
         <f t="shared" si="4"/>
-        <v>36</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="R6">
+        <v>16560</v>
+      </c>
+      <c r="S6">
         <f t="shared" si="5"/>
-        <v>16560</v>
-      </c>
-      <c r="S6">
-        <f t="shared" si="6"/>
         <v>8478720</v>
       </c>
       <c r="U6">
@@ -4759,19 +4882,19 @@
         <v>47</v>
       </c>
       <c r="X6">
+        <f t="shared" si="6"/>
+        <v>1410</v>
+      </c>
+      <c r="Z6">
         <f t="shared" si="7"/>
-        <v>1410</v>
-      </c>
-      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AA6">
+        <v>23</v>
+      </c>
+      <c r="AB6">
         <f t="shared" si="9"/>
-        <v>23</v>
-      </c>
-      <c r="AB6">
-        <f t="shared" si="10"/>
         <v>30</v>
       </c>
       <c r="AD6" s="52">
@@ -4780,7 +4903,7 @@
       </c>
       <c r="AE6" s="50"/>
       <c r="AF6" s="56">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>721920</v>
       </c>
     </row>
@@ -4822,7 +4945,7 @@
         <v>20</v>
       </c>
       <c r="L7" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>56.194999999999709</v>
       </c>
       <c r="N7" s="49"/>
@@ -4848,15 +4971,15 @@
         <v>3832.5</v>
       </c>
       <c r="Z7" s="49">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="AA7" s="49">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="AA7" s="49">
+        <v>3</v>
+      </c>
+      <c r="AB7" s="49">
         <f t="shared" si="9"/>
-        <v>3</v>
-      </c>
-      <c r="AB7" s="49">
-        <f t="shared" si="10"/>
         <v>52.5</v>
       </c>
       <c r="AD7" s="53">
@@ -4907,7 +5030,7 @@
         <v>52</v>
       </c>
       <c r="L8" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>28.926768133839687</v>
       </c>
       <c r="N8" s="49"/>
@@ -4933,15 +5056,15 @@
         <v>1719.4257762404284</v>
       </c>
       <c r="Z8" s="49">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA8" s="49">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AA8" s="49">
+        <v>28</v>
+      </c>
+      <c r="AB8" s="49">
         <f t="shared" si="9"/>
-        <v>28</v>
-      </c>
-      <c r="AB8" s="49">
-        <f t="shared" si="10"/>
         <v>39.425776240428377</v>
       </c>
       <c r="AD8" s="53">
@@ -4999,26 +5122,26 @@
         <v>52</v>
       </c>
       <c r="L10" s="48">
+        <f t="shared" si="11"/>
+        <v>18.849999999998545</v>
+      </c>
+      <c r="N10">
         <f t="shared" si="2"/>
-        <v>18.849999999998545</v>
-      </c>
-      <c r="N10">
+        <v>7</v>
+      </c>
+      <c r="O10">
         <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="O10">
+        <v>52</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="R10">
         <f t="shared" si="4"/>
-        <v>52</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="R10">
+        <v>28320</v>
+      </c>
+      <c r="S10">
         <f t="shared" si="5"/>
-        <v>28320</v>
-      </c>
-      <c r="S10">
-        <f t="shared" si="6"/>
         <v>14499840</v>
       </c>
       <c r="U10">
@@ -5032,15 +5155,15 @@
         <v>3960</v>
       </c>
       <c r="Z10">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="AA10">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="AA10">
+        <v>6</v>
+      </c>
+      <c r="AB10">
         <f t="shared" si="9"/>
-        <v>6</v>
-      </c>
-      <c r="AB10">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AD10" s="52">
@@ -5049,7 +5172,7 @@
       </c>
       <c r="AE10" s="50"/>
       <c r="AF10" s="56">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>2027520</v>
       </c>
     </row>
@@ -5085,26 +5208,26 @@
         <v>3</v>
       </c>
       <c r="L11" s="48">
+        <f t="shared" si="11"/>
+        <v>0.38999999999941792</v>
+      </c>
+      <c r="N11">
         <f t="shared" si="2"/>
-        <v>0.38999999999941792</v>
-      </c>
-      <c r="N11">
+        <v>7</v>
+      </c>
+      <c r="O11">
         <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="R11">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="R11">
+        <v>25200</v>
+      </c>
+      <c r="S11">
         <f t="shared" si="5"/>
-        <v>25200</v>
-      </c>
-      <c r="S11">
-        <f t="shared" si="6"/>
         <v>12902400</v>
       </c>
       <c r="U11">
@@ -5118,15 +5241,15 @@
         <v>2970</v>
       </c>
       <c r="Z11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA11">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AA11">
+        <v>49</v>
+      </c>
+      <c r="AB11">
         <f t="shared" si="9"/>
-        <v>49</v>
-      </c>
-      <c r="AB11">
-        <f t="shared" si="10"/>
         <v>30</v>
       </c>
       <c r="AD11" s="52">
@@ -5135,7 +5258,7 @@
       </c>
       <c r="AE11" s="50"/>
       <c r="AF11" s="56">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1520640</v>
       </c>
     </row>
@@ -5171,26 +5294,26 @@
         <v>3</v>
       </c>
       <c r="L12" s="48">
+        <f t="shared" si="11"/>
+        <v>58.290000000000873</v>
+      </c>
+      <c r="N12">
         <f t="shared" si="2"/>
-        <v>58.290000000000873</v>
-      </c>
-      <c r="N12">
+        <v>10</v>
+      </c>
+      <c r="O12">
         <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="R12">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="R12">
+        <v>36000</v>
+      </c>
+      <c r="S12">
         <f t="shared" si="5"/>
-        <v>36000</v>
-      </c>
-      <c r="S12">
-        <f t="shared" si="6"/>
         <v>18432000</v>
       </c>
       <c r="U12">
@@ -5204,15 +5327,15 @@
         <v>1020</v>
       </c>
       <c r="Z12">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA12">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AA12">
+        <v>17</v>
+      </c>
+      <c r="AB12">
         <f t="shared" si="9"/>
-        <v>17</v>
-      </c>
-      <c r="AB12">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AD12" s="52">
@@ -5221,7 +5344,7 @@
       </c>
       <c r="AE12" s="50"/>
       <c r="AF12" s="56">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>522240</v>
       </c>
     </row>
@@ -5257,26 +5380,26 @@
         <v>58</v>
       </c>
       <c r="L13" s="48">
+        <f t="shared" si="11"/>
+        <v>49.279999999998836</v>
+      </c>
+      <c r="N13">
         <f t="shared" si="2"/>
-        <v>49.279999999998836</v>
-      </c>
-      <c r="N13">
+        <v>7</v>
+      </c>
+      <c r="O13">
         <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="O13">
+        <v>56</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="R13">
         <f t="shared" si="4"/>
-        <v>56</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="R13">
+        <v>28560</v>
+      </c>
+      <c r="S13">
         <f t="shared" si="5"/>
-        <v>28560</v>
-      </c>
-      <c r="S13">
-        <f t="shared" si="6"/>
         <v>14622720</v>
       </c>
       <c r="U13">
@@ -5290,15 +5413,15 @@
         <v>1230</v>
       </c>
       <c r="Z13">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA13">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AA13">
+        <v>20</v>
+      </c>
+      <c r="AB13">
         <f t="shared" si="9"/>
-        <v>20</v>
-      </c>
-      <c r="AB13">
-        <f t="shared" si="10"/>
         <v>30</v>
       </c>
       <c r="AD13" s="52">
@@ -5307,7 +5430,7 @@
       </c>
       <c r="AE13" s="50"/>
       <c r="AF13" s="56">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>629760</v>
       </c>
     </row>
@@ -5343,26 +5466,26 @@
         <v>16</v>
       </c>
       <c r="L14" s="48">
+        <f t="shared" si="11"/>
+        <v>39.630000000001019</v>
+      </c>
+      <c r="N14">
         <f t="shared" si="2"/>
-        <v>39.630000000001019</v>
-      </c>
-      <c r="N14">
+        <v>6</v>
+      </c>
+      <c r="O14">
         <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="O14">
+        <v>16</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="R14">
         <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-      <c r="R14">
+        <v>22560</v>
+      </c>
+      <c r="S14">
         <f t="shared" si="5"/>
-        <v>22560</v>
-      </c>
-      <c r="S14">
-        <f t="shared" si="6"/>
         <v>11550720</v>
       </c>
       <c r="U14">
@@ -5376,15 +5499,15 @@
         <v>1770</v>
       </c>
       <c r="Z14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA14">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AA14">
+        <v>29</v>
+      </c>
+      <c r="AB14">
         <f t="shared" si="9"/>
-        <v>29</v>
-      </c>
-      <c r="AB14">
-        <f t="shared" si="10"/>
         <v>30</v>
       </c>
       <c r="AD14" s="52">
@@ -5393,7 +5516,7 @@
       </c>
       <c r="AE14" s="50"/>
       <c r="AF14" s="56">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>906240</v>
       </c>
     </row>
@@ -5435,7 +5558,7 @@
         <v>50</v>
       </c>
       <c r="L15" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>57.288000000000466</v>
       </c>
       <c r="N15" s="49"/>
@@ -5461,15 +5584,15 @@
         <v>2190</v>
       </c>
       <c r="Z15" s="49">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA15" s="49">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AA15" s="49">
+        <v>36</v>
+      </c>
+      <c r="AB15" s="49">
         <f t="shared" si="9"/>
-        <v>36</v>
-      </c>
-      <c r="AB15" s="49">
-        <f t="shared" si="10"/>
         <v>30</v>
       </c>
       <c r="AD15" s="53">
@@ -5520,7 +5643,7 @@
         <v>25</v>
       </c>
       <c r="L16" s="48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4.2006690391808661</v>
       </c>
       <c r="N16" s="49"/>
@@ -5546,15 +5669,15 @@
         <v>1245.8129875707671</v>
       </c>
       <c r="Z16" s="49">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA16" s="49">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AA16" s="49">
+        <v>20</v>
+      </c>
+      <c r="AB16" s="49">
         <f t="shared" si="9"/>
-        <v>20</v>
-      </c>
-      <c r="AB16" s="49">
-        <f t="shared" si="10"/>
         <v>45.812987570767064</v>
       </c>
       <c r="AD16" s="53">
@@ -5603,22 +5726,22 @@
         <v>22</v>
       </c>
       <c r="L18" s="48">
+        <f t="shared" si="11"/>
+        <v>59.600000000000364</v>
+      </c>
+      <c r="N18">
         <f t="shared" si="2"/>
-        <v>59.600000000000364</v>
-      </c>
-      <c r="N18">
+        <v>3</v>
+      </c>
+      <c r="O18">
         <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="O18">
+        <v>20</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="R18">
         <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="R18">
-        <f t="shared" si="5"/>
         <v>12000</v>
       </c>
       <c r="U18">
@@ -5632,15 +5755,15 @@
         <v>660</v>
       </c>
       <c r="Z18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA18">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AA18">
+        <v>11</v>
+      </c>
+      <c r="AB18">
         <f t="shared" si="9"/>
-        <v>11</v>
-      </c>
-      <c r="AB18">
-        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AD18" s="52">
@@ -5648,21 +5771,172 @@
         <v>5.5E-2</v>
       </c>
       <c r="AF18" s="56">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>337920</v>
       </c>
     </row>
     <row r="20" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="J20" s="63" t="s">
+      <c r="J20" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="K20" s="63"/>
-      <c r="L20" s="63"/>
-      <c r="N20" s="63" t="s">
+      <c r="K20" s="65"/>
+      <c r="L20" s="65"/>
+      <c r="N20" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="O20" s="63"/>
-      <c r="P20" s="63"/>
+      <c r="O20" s="65"/>
+      <c r="P20" s="65"/>
+    </row>
+    <row r="23" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="S23">
+        <v>30960</v>
+      </c>
+      <c r="X23">
+        <v>3810</v>
+      </c>
+      <c r="AD23">
+        <v>0.12306201550387597</v>
+      </c>
+    </row>
+    <row r="24" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="S24">
+        <v>27120</v>
+      </c>
+      <c r="X24">
+        <v>5130</v>
+      </c>
+      <c r="AD24">
+        <v>0.18915929203539822</v>
+      </c>
+    </row>
+    <row r="25" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="S25">
+        <v>30720</v>
+      </c>
+      <c r="X25">
+        <v>4980</v>
+      </c>
+      <c r="AD25">
+        <v>0.162109375</v>
+      </c>
+    </row>
+    <row r="26" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="S26">
+        <v>16560</v>
+      </c>
+      <c r="X26">
+        <v>1410</v>
+      </c>
+      <c r="AD26">
+        <v>8.5144927536231887E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="S27">
+        <v>26340</v>
+      </c>
+      <c r="X27">
+        <v>3832.5</v>
+      </c>
+      <c r="AD27">
+        <v>0.13986890251887651</v>
+      </c>
+    </row>
+    <row r="28" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="S28">
+        <v>6752.4217877736282</v>
+      </c>
+      <c r="X28">
+        <v>1719.4257762404284</v>
+      </c>
+      <c r="AD28">
+        <v>4.5465613394117844E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="S30">
+        <v>28320</v>
+      </c>
+      <c r="X30">
+        <v>3960</v>
+      </c>
+      <c r="AD30">
+        <v>0.13983050847457626</v>
+      </c>
+    </row>
+    <row r="31" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="S31">
+        <v>25200</v>
+      </c>
+      <c r="X31">
+        <v>2970</v>
+      </c>
+      <c r="AD31">
+        <v>0.11785714285714285</v>
+      </c>
+    </row>
+    <row r="32" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="S32">
+        <v>36000</v>
+      </c>
+      <c r="X32">
+        <v>1020</v>
+      </c>
+      <c r="AD32">
+        <v>2.8333333333333332E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="19:30" x14ac:dyDescent="0.25">
+      <c r="S33">
+        <v>28560</v>
+      </c>
+      <c r="X33">
+        <v>1230</v>
+      </c>
+      <c r="AD33">
+        <v>4.3067226890756302E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="19:30" x14ac:dyDescent="0.25">
+      <c r="S34">
+        <v>22560</v>
+      </c>
+      <c r="X34">
+        <v>1770</v>
+      </c>
+      <c r="AD34">
+        <v>7.8457446808510634E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="19:30" x14ac:dyDescent="0.25">
+      <c r="S35">
+        <v>28128</v>
+      </c>
+      <c r="X35">
+        <v>2190</v>
+      </c>
+      <c r="AD35">
+        <v>8.1509131672863874E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="19:30" x14ac:dyDescent="0.25">
+      <c r="S36">
+        <v>5043.9984139569278</v>
+      </c>
+      <c r="X36">
+        <v>1245.8129875707671</v>
+      </c>
+      <c r="AD36">
+        <v>4.7532408054752874E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="19:30" x14ac:dyDescent="0.25">
+      <c r="X38">
+        <v>660</v>
+      </c>
+      <c r="AD38">
+        <v>5.5E-2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6199,7 +6473,7 @@
   <dimension ref="A1:Z16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I16"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6880,15 +7154,18 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -6908,13 +7185,13 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
       <c r="H2" s="62"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -6930,11 +7207,19 @@
       <c r="G3" s="57">
         <v>4.4097222222222225E-2</v>
       </c>
-      <c r="H3" s="62">
+      <c r="H3" s="64">
         <v>12.306201550387597</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <f>C3/(512*30)</f>
+        <v>1032</v>
+      </c>
+      <c r="K3">
+        <f>F3/(30*512)</f>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>19</v>
       </c>
@@ -6950,11 +7235,19 @@
       <c r="G4" s="57">
         <v>5.9375000000000004E-2</v>
       </c>
-      <c r="H4" s="62">
+      <c r="H4" s="64">
         <v>18.915929203539822</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <f t="shared" ref="J4:J14" si="0">C4/(512*30)</f>
+        <v>904</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K14" si="1">F4/(30*512)</f>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>29</v>
       </c>
@@ -6970,11 +7263,19 @@
       <c r="G5" s="57">
         <v>5.7638888888888885E-2</v>
       </c>
-      <c r="H5" s="62">
+      <c r="H5" s="64">
         <v>16.2109375</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>1024</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>32</v>
       </c>
@@ -6990,11 +7291,19 @@
       <c r="G6" s="57">
         <v>1.5972222222222224E-2</v>
       </c>
-      <c r="H6" s="62">
+      <c r="H6" s="64">
         <v>8.5144927536231894</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <f>C6/(512*30)</f>
+        <v>552</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -7010,11 +7319,19 @@
       <c r="G7" s="57">
         <v>4.4363425925925924E-2</v>
       </c>
-      <c r="H7" s="62">
+      <c r="H7" s="64">
         <v>13.986890251887651</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7" s="60">
+        <f>AVERAGE(J3:J6)</f>
+        <v>878</v>
+      </c>
+      <c r="K7" s="60">
+        <f>AVERAGE(K3:K6)</f>
+        <v>127.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>54</v>
       </c>
@@ -7030,19 +7347,31 @@
       <c r="G8" s="57">
         <v>1.9895833333333331E-2</v>
       </c>
-      <c r="H8" s="62">
+      <c r="H8" s="64">
         <v>4.5465613394117845</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <f>STDEV(J3:J6)</f>
+        <v>225.08072625912095</v>
+      </c>
+      <c r="K8">
+        <f>STDEV(K3:K6)</f>
+        <v>57.314192541347616</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
       <c r="C9" s="60"/>
       <c r="F9" s="60"/>
-      <c r="H9" s="62"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" s="64"/>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>35</v>
       </c>
@@ -7058,11 +7387,19 @@
       <c r="G10" s="57">
         <v>4.5833333333333337E-2</v>
       </c>
-      <c r="H10" s="62">
+      <c r="H10" s="64">
         <v>13.983050847457626</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>944</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>37</v>
       </c>
@@ -7078,11 +7415,19 @@
       <c r="G11" s="57">
         <v>3.4374999999999996E-2</v>
       </c>
-      <c r="H11" s="62">
+      <c r="H11" s="64">
         <v>11.785714285714285</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>840</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>43</v>
       </c>
@@ -7098,11 +7443,19 @@
       <c r="G12" s="57">
         <v>1.1805555555555555E-2</v>
       </c>
-      <c r="H12" s="62">
+      <c r="H12" s="64">
         <v>2.833333333333333</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>1200</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>45</v>
       </c>
@@ -7118,11 +7471,19 @@
       <c r="G13" s="57">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="H13" s="62">
+      <c r="H13" s="64">
         <v>4.3067226890756301</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>952</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>47</v>
       </c>
@@ -7138,11 +7499,19 @@
       <c r="G14" s="57">
         <v>2.0486111111111111E-2</v>
       </c>
-      <c r="H14" s="62">
+      <c r="H14" s="64">
         <v>7.8457446808510634</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>752</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>23</v>
       </c>
@@ -7158,11 +7527,19 @@
       <c r="G15" s="57">
         <v>2.5347222222222219E-2</v>
       </c>
-      <c r="H15" s="62">
+      <c r="H15" s="64">
         <v>8.1509131672863866</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <f>AVERAGE(J10:J14)</f>
+        <v>937.6</v>
+      </c>
+      <c r="K15">
+        <f>AVERAGE(K10:K14)</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>54</v>
       </c>
@@ -7178,8 +7555,16 @@
       <c r="G16" s="57">
         <v>1.4421296296296295E-2</v>
       </c>
-      <c r="H16" s="62">
+      <c r="H16" s="64">
         <v>4.7532408054752873</v>
+      </c>
+      <c r="J16">
+        <f>STDEV(J10:J14)</f>
+        <v>168.13328046523105</v>
+      </c>
+      <c r="K16">
+        <f>STDEV(K10:K14)</f>
+        <v>41.527099585692234</v>
       </c>
     </row>
   </sheetData>
@@ -7190,35 +7575,50 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:T1048576"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>75</v>
       </c>
       <c r="E1" t="s">
         <v>76</v>
       </c>
-      <c r="H1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H1" s="70" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="70"/>
+      <c r="N1" s="70" t="s">
+        <v>83</v>
+      </c>
+      <c r="O1" s="70"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>23</v>
       </c>
@@ -7232,174 +7632,861 @@
         <v>54</v>
       </c>
       <c r="H2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K2" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>89</v>
+      </c>
+      <c r="P2" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>90</v>
+      </c>
+      <c r="R2" t="s">
+        <v>91</v>
+      </c>
+      <c r="S2" t="s">
+        <v>92</v>
+      </c>
+      <c r="T2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="48">
         <v>65.25</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="48">
         <v>12.36595</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="48">
         <v>68</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="48">
         <v>4.1231059999999999</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="63">
         <v>0.90476190000000001</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="48">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="48">
+        <v>-1.5</v>
+      </c>
+      <c r="K3" s="48">
+        <v>-21</v>
+      </c>
+      <c r="L3" s="48">
+        <v>13</v>
+      </c>
+      <c r="N3" s="63">
+        <v>0.69458940000000002</v>
+      </c>
+      <c r="O3" s="48">
+        <v>-0.42621999999999999</v>
+      </c>
+      <c r="P3" s="48">
+        <v>3.5363739999999999</v>
+      </c>
+      <c r="Q3" s="48">
+        <v>65.25</v>
+      </c>
+      <c r="R3" s="48">
+        <v>68</v>
+      </c>
+      <c r="S3" s="48">
+        <v>-21.629149999999999</v>
+      </c>
+      <c r="T3" s="48">
+        <v>16.129149999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
+        <v>84</v>
+      </c>
+      <c r="B4" s="48">
         <v>11.25</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="48">
         <v>7.4105780000000001</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="48">
         <v>8.4</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="48">
         <v>2.19089</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="63">
         <v>0.79716969999999998</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="48">
         <v>11.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="48">
+        <v>1.4727889999999999E-5</v>
+      </c>
+      <c r="K4" s="48">
+        <v>-4.0000679999999997</v>
+      </c>
+      <c r="L4" s="48">
+        <v>13.99999</v>
+      </c>
+      <c r="N4" s="63">
+        <v>0.50489709999999999</v>
+      </c>
+      <c r="O4" s="48">
+        <v>0.74361180000000004</v>
+      </c>
+      <c r="P4" s="48">
+        <v>3.4216660000000001</v>
+      </c>
+      <c r="Q4" s="48">
+        <v>11.25</v>
+      </c>
+      <c r="R4" s="48">
+        <v>8.4</v>
+      </c>
+      <c r="S4" s="48">
+        <v>-8.5394050000000004</v>
+      </c>
+      <c r="T4" s="48">
+        <v>14.2394</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="48">
         <v>111.5</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="48">
         <v>6.5574389999999996</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="48">
         <v>93</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="48">
         <v>11.42366</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="63">
         <v>3.1746030000000001E-2</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="48">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="48">
+        <v>21</v>
+      </c>
+      <c r="K5" s="48">
+        <v>2</v>
+      </c>
+      <c r="L5" s="48">
+        <v>33</v>
+      </c>
+      <c r="N5" s="63">
+        <v>2.0419610000000001E-2</v>
+      </c>
+      <c r="O5" s="48">
+        <v>3.0475650000000001</v>
+      </c>
+      <c r="P5" s="48">
+        <v>6.5027340000000002</v>
+      </c>
+      <c r="Q5" s="48">
+        <v>111.5</v>
+      </c>
+      <c r="R5" s="48">
+        <v>93</v>
+      </c>
+      <c r="S5" s="48">
+        <v>3.9201920000000001</v>
+      </c>
+      <c r="T5" s="48">
+        <v>33.079810000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="48">
         <v>29</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="48">
         <v>1.154701</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="48">
         <v>27.8</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="48">
         <v>1.643168</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="63">
         <v>0.3661566</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="48">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="48">
+        <v>1.000041</v>
+      </c>
+      <c r="K6" s="48">
+        <v>-1</v>
+      </c>
+      <c r="L6" s="48">
+        <v>4.999911</v>
+      </c>
+      <c r="N6" s="63">
+        <v>0.24033099999999999</v>
+      </c>
+      <c r="O6" s="48">
+        <v>1.2840769999999999</v>
+      </c>
+      <c r="P6" s="48">
+        <v>6.9377079999999998</v>
+      </c>
+      <c r="Q6" s="48">
+        <v>29</v>
+      </c>
+      <c r="R6" s="48">
+        <v>27.8</v>
+      </c>
+      <c r="S6" s="48">
+        <v>-1.0138240000000001</v>
+      </c>
+      <c r="T6" s="48">
+        <v>3.413824</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>55</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="48">
         <v>20.25</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="48">
         <v>6.0759090000000002</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="48">
         <v>20.5</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="48">
         <v>1</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="63">
         <v>0.30052230000000002</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="48">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="48">
+        <v>-1.9999579999999999</v>
+      </c>
+      <c r="K7" s="48">
+        <v>-6.999905</v>
+      </c>
+      <c r="L7" s="48">
+        <v>9</v>
+      </c>
+      <c r="N7" s="63">
+        <v>0.94015159999999998</v>
+      </c>
+      <c r="O7" s="48">
+        <v>-8.1199789999999994E-2</v>
+      </c>
+      <c r="P7" s="48">
+        <v>3.1624089999999998</v>
+      </c>
+      <c r="Q7" s="48">
+        <v>20.25</v>
+      </c>
+      <c r="R7" s="48">
+        <v>20.5</v>
+      </c>
+      <c r="S7" s="48">
+        <v>-9.7695880000000006</v>
+      </c>
+      <c r="T7" s="48">
+        <v>9.2695880000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8">
-        <v>0.25</v>
-      </c>
-      <c r="C8">
-        <v>0.5</v>
-      </c>
-      <c r="E8">
-        <v>0.2</v>
-      </c>
-      <c r="F8">
-        <v>0.44721359999999999</v>
-      </c>
-      <c r="H8">
+        <v>57</v>
+      </c>
+      <c r="B8" s="48">
+        <v>5.75</v>
+      </c>
+      <c r="C8" s="48">
+        <v>5.909033</v>
+      </c>
+      <c r="E8" s="48">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F8" s="48">
+        <v>3.6469170000000002</v>
+      </c>
+      <c r="H8" s="63">
+        <v>0.90476190000000001</v>
+      </c>
+      <c r="I8" s="48">
+        <v>11</v>
+      </c>
+      <c r="J8" s="48">
+        <v>1.5</v>
+      </c>
+      <c r="K8" s="48">
+        <v>-6</v>
+      </c>
+      <c r="L8" s="48">
+        <v>12</v>
+      </c>
+      <c r="N8" s="63">
+        <v>0.70640389999999997</v>
+      </c>
+      <c r="O8" s="48">
+        <v>0.40002559999999998</v>
+      </c>
+      <c r="P8" s="48">
+        <v>4.7744200000000001</v>
+      </c>
+      <c r="Q8" s="48">
+        <v>5.75</v>
+      </c>
+      <c r="R8" s="48">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="S8" s="48">
+        <v>-7.4499029999999999</v>
+      </c>
+      <c r="T8" s="48">
+        <v>10.149900000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="H9" s="63"/>
+      <c r="N9" s="63"/>
+      <c r="O9" s="48"/>
+      <c r="P9" s="48"/>
+      <c r="Q9" s="48"/>
+      <c r="R9" s="48"/>
+      <c r="S9" s="48"/>
+      <c r="T9" s="48"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="48">
+        <v>26340</v>
+      </c>
+      <c r="C10" s="48">
+        <v>6752.4219999999996</v>
+      </c>
+      <c r="E10" s="48">
+        <v>28128</v>
+      </c>
+      <c r="F10" s="48">
+        <v>5043.9979999999996</v>
+      </c>
+      <c r="H10" s="63">
         <v>1</v>
       </c>
-      <c r="I8">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9">
-        <v>5.75</v>
-      </c>
-      <c r="C9">
-        <v>5.909033</v>
-      </c>
-      <c r="E9">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="F9">
-        <v>3.6469170000000002</v>
-      </c>
-      <c r="H9">
+      <c r="I10" s="48">
+        <v>10</v>
+      </c>
+      <c r="J10" s="48">
+        <v>360</v>
+      </c>
+      <c r="K10" s="48">
+        <v>-12000</v>
+      </c>
+      <c r="L10" s="48">
+        <v>8160</v>
+      </c>
+      <c r="N10" s="63">
+        <v>0.67657800000000001</v>
+      </c>
+      <c r="O10" s="48">
+        <v>-0.44034620000000002</v>
+      </c>
+      <c r="P10" s="48">
+        <v>5.4601550000000003</v>
+      </c>
+      <c r="Q10" s="48">
+        <v>26340</v>
+      </c>
+      <c r="R10" s="48">
+        <v>28128</v>
+      </c>
+      <c r="S10" s="48">
+        <v>-11966.59</v>
+      </c>
+      <c r="T10" s="48">
+        <v>8390.59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="48">
+        <v>3832.5</v>
+      </c>
+      <c r="C11" s="48">
+        <v>1719.4259999999999</v>
+      </c>
+      <c r="E11" s="48">
+        <v>2190</v>
+      </c>
+      <c r="F11" s="48">
+        <v>1245.8130000000001</v>
+      </c>
+      <c r="H11" s="63">
+        <v>0.19047620000000001</v>
+      </c>
+      <c r="I11" s="48">
+        <v>16</v>
+      </c>
+      <c r="J11" s="48">
+        <v>2025</v>
+      </c>
+      <c r="K11" s="48">
+        <v>-1560</v>
+      </c>
+      <c r="L11" s="48">
+        <v>3960</v>
+      </c>
+      <c r="N11" s="63">
+        <v>0.1660336</v>
+      </c>
+      <c r="O11" s="48">
+        <v>1.6032850000000001</v>
+      </c>
+      <c r="P11" s="48">
+        <v>5.3423100000000003</v>
+      </c>
+      <c r="Q11" s="48">
+        <v>3832.5</v>
+      </c>
+      <c r="R11" s="48">
+        <v>2190</v>
+      </c>
+      <c r="S11" s="48">
+        <v>-941.00300000000004</v>
+      </c>
+      <c r="T11" s="48">
+        <v>4226.0029999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="71">
+        <v>0.13986889999999999</v>
+      </c>
+      <c r="C12" s="71">
+        <v>4.5465609999999997E-2</v>
+      </c>
+      <c r="E12" s="71">
+        <v>8.1509129999999999E-2</v>
+      </c>
+      <c r="F12" s="71">
+        <v>4.7532409999999997E-2</v>
+      </c>
+      <c r="H12" s="63">
+        <v>0.1111111</v>
+      </c>
+      <c r="I12" s="48">
+        <v>17</v>
+      </c>
+      <c r="J12" s="71">
+        <v>5.3070190000000003E-2</v>
+      </c>
+      <c r="K12" s="71">
+        <v>-3.271222E-2</v>
+      </c>
+      <c r="L12" s="71">
+        <v>0.1460921</v>
+      </c>
+      <c r="N12" s="63">
+        <v>0.1047902</v>
+      </c>
+      <c r="O12" s="48">
+        <v>1.8751279999999999</v>
+      </c>
+      <c r="P12" s="48">
+        <v>6.6987940000000004</v>
+      </c>
+      <c r="Q12" s="71">
+        <v>0.13986889999999999</v>
+      </c>
+      <c r="R12" s="71">
+        <v>8.1509129999999999E-2</v>
+      </c>
+      <c r="S12" s="71">
+        <v>-1.5910790000000001E-2</v>
+      </c>
+      <c r="T12" s="71">
+        <v>0.13263030000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R13" s="48"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14">
+        <f>INT(B10/(60*60))</f>
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:T14" si="0">INT(C10/(60*60))</f>
         <v>1</v>
       </c>
-      <c r="I9">
-        <v>10.5</v>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15">
+        <f>INT((B10-60*60*B14)/60)</f>
+        <v>19</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:T15" si="1">INT((C10-60*60*C14)/60)</f>
+        <v>52</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="48">
+        <f>B10-60*60*B14-60*B15</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="48">
+        <f t="shared" ref="C16:T16" si="2">C10-60*60*C14-60*C15</f>
+        <v>32.421999999999571</v>
+      </c>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="F16" s="48">
+        <f t="shared" si="2"/>
+        <v>3.9979999999995925</v>
+      </c>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="48">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="48">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="48">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="48"/>
+      <c r="N16" s="48"/>
+      <c r="O16" s="48"/>
+      <c r="P16" s="48"/>
+      <c r="Q16" s="48">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R16" s="48">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="S16" s="48">
+        <f t="shared" si="2"/>
+        <v>33.409999999999854</v>
+      </c>
+      <c r="T16" s="48">
+        <f t="shared" si="2"/>
+        <v>50.590000000000146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18">
+        <f>INT(B11/(60*60))</f>
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:T18" si="3">INT(C11/(60*60))</f>
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19">
+        <f>INT((B11-60*60*B18)/60)</f>
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ref="C19:T19" si="4">INT((C11-60*60*C18)/60)</f>
+        <v>28</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="4"/>
+        <v>33</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="4"/>
+        <v>34</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="4"/>
+        <v>44</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="48">
+        <f>B11-60*60*B18-60*B19</f>
+        <v>52.5</v>
+      </c>
+      <c r="C20" s="48">
+        <f t="shared" ref="C20:T20" si="5">C11-60*60*C18-60*C19</f>
+        <v>39.425999999999931</v>
+      </c>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="F20" s="48">
+        <f t="shared" si="5"/>
+        <v>45.813000000000102</v>
+      </c>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="48">
+        <f t="shared" si="5"/>
+        <v>45</v>
+      </c>
+      <c r="K20" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L20" s="48">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="48"/>
+      <c r="P20" s="48"/>
+      <c r="Q20" s="48">
+        <f t="shared" si="5"/>
+        <v>52.5</v>
+      </c>
+      <c r="R20" s="48">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="S20" s="48">
+        <f t="shared" si="5"/>
+        <v>18.996999999999844</v>
+      </c>
+      <c r="T20" s="48">
+        <f t="shared" si="5"/>
+        <v>26.002999999999702</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="N1:O1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="H3:H12">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:N12">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>